<commit_message>
search photo command can now search photos for all cars of the set
</commit_message>
<xml_diff>
--- a/log avalabilityes.xlsx
+++ b/log avalabilityes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Billy\Douments\Self made programs\Melbourne-transport-discord-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A40F97-DDFD-4C2A-A1F3-F56D76CF4FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294CC545-C78B-4BA4-A4D8-992D7A852527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{F3EDBA5E-8EA3-4903-824E-2BA2D9471524}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
   <si>
     <t>Mode</t>
   </si>
@@ -96,16 +96,102 @@
   </si>
   <si>
     <t>✅^</t>
+  </si>
+  <si>
+    <t>TrackPulse VIC</t>
+  </si>
+  <si>
+    <t>Bot Comparison</t>
+  </si>
+  <si>
+    <t>VPT Bot</t>
+  </si>
+  <si>
+    <t>trainbot</t>
+  </si>
+  <si>
+    <t>Train Line Status</t>
+  </si>
+  <si>
+    <t>Bus and Tram Line Status</t>
+  </si>
+  <si>
+    <t>Station Departures</t>
+  </si>
+  <si>
+    <t>Train search</t>
+  </si>
+  <si>
+    <t>Train Photo</t>
+  </si>
+  <si>
+    <t>Train Runs and Location</t>
+  </si>
+  <si>
+    <r>
+      <t>⚠</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> runs only</t>
+    </r>
+  </si>
+  <si>
+    <t>Log feature</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">⚠ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>metro trains only</t>
+    </r>
+  </si>
+  <si>
+    <t>Detailed log stats</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Tram search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,8 +217,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,20 +554,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D67BF17-4F47-4C6C-9ACD-0DD836590FCB}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -494,7 +589,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -507,8 +602,17 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -521,8 +625,20 @@
       <c r="E4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -535,8 +651,20 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -549,8 +677,20 @@
       <c r="E6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -563,8 +703,20 @@
       <c r="E7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -577,8 +729,20 @@
       <c r="E8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -591,8 +755,20 @@
       <c r="E9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -605,18 +781,69 @@
       <c r="E10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>